<commit_message>
Integrated statistics page data and the database
</commit_message>
<xml_diff>
--- a/db-backup/MockData.xlsx
+++ b/db-backup/MockData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Egyetem_PTI\Diplomamunka\thesis-dms\db-backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{20C343D2-179B-4209-8BD7-964E79DDECA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CD213154-26EE-484D-9714-60045896DC77}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{20C343D2-179B-4209-8BD7-964E79DDECA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{554B84A8-4EBB-4FF5-A5D6-4AA4735B7A66}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="24825" activeTab="3" xr2:uid="{CCBAF8E0-E5E1-4B4B-975B-45441D02614E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="24825" xr2:uid="{CCBAF8E0-E5E1-4B4B-975B-45441D02614E}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -883,8 +883,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="6">
-        <v>44115.818599189108</v>
+        <v>44501.930338049555</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="6">
-        <v>44128.014224246806</v>
+        <v>44472.802439237697</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="6">
-        <v>44200.421501476012</v>
+        <v>44513.343538625973</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="6">
-        <v>44308.068148349521</v>
+        <v>44521.989396953293</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="6">
-        <v>44281.048023435855</v>
+        <v>44486.057613471581</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="6">
-        <v>44294.597271296167</v>
+        <v>44501.326610148702</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="6">
-        <v>44212.746958006988</v>
+        <v>44476.374774090182</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="6">
-        <v>44141.727157351161</v>
+        <v>44477.440468538873</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1175,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="I10" s="6">
-        <v>44173.993280170827</v>
+        <v>44503.603599975322</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="I11" s="6">
-        <v>44302.245353179096</v>
+        <v>44527.719434979161</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="6">
-        <v>44132.995508546948</v>
+        <v>44494.242658962656</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="6">
-        <v>44196.705618940759</v>
+        <v>44489.865231722142</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="6">
-        <v>44145.383308061952</v>
+        <v>44484.401002294944</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="6">
-        <v>44136.004881543187</v>
+        <v>44533.324179729978</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="6">
-        <v>44311.156425894696</v>
+        <v>44531.099656801853</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="6">
-        <v>44220.924590939227</v>
+        <v>44491.122377506152</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="6">
-        <v>44207.749838560543</v>
+        <v>44480.570100457226</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="6">
-        <v>44191.405834515812</v>
+        <v>44496.743357915788</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="6">
-        <v>44153.517143886638</v>
+        <v>44496.899970593353</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="6">
-        <v>44075.877151942688</v>
+        <v>44471.450583982405</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="I22" s="6">
-        <v>44282.505521778716</v>
+        <v>44481.435805008354</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="6">
-        <v>44248.479681168887</v>
+        <v>44520.658584588135</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="6">
-        <v>44247.043955733781</v>
+        <v>44495.456741345137</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="6">
-        <v>44255.596385722107</v>
+        <v>44531.306088241407</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="6">
-        <v>44225.309198868366</v>
+        <v>44504.084114718993</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="6">
-        <v>44155.831883141698</v>
+        <v>44518.526148117977</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>3</v>
       </c>
       <c r="I28" s="6">
-        <v>44224.253216504738</v>
+        <v>44476.496937731135</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="6">
-        <v>44201.255031124754</v>
+        <v>44470.668257442667</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>3</v>
       </c>
       <c r="I30" s="6">
-        <v>44171.542462069468</v>
+        <v>44487.796635433093</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>3</v>
       </c>
       <c r="I31" s="6">
-        <v>44263.673191406691</v>
+        <v>44478.817663571252</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="6">
-        <v>44236.893111824822</v>
+        <v>44502.868772477348</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="6">
-        <v>44156.907635241572</v>
+        <v>44509.903712374813</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>4</v>
       </c>
       <c r="I34" s="6">
-        <v>44256.065052154147</v>
+        <v>44482.464790495033</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="6">
-        <v>44213.876205599845</v>
+        <v>44471.845028533993</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>4</v>
       </c>
       <c r="I36" s="6">
-        <v>44152.467248479043</v>
+        <v>44523.35006640161</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="6">
-        <v>44083.81964372834</v>
+        <v>44504.722729689849</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="6">
-        <v>44320.143903487711</v>
+        <v>44498.270922131152</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="6">
-        <v>44233.14719919963</v>
+        <v>44487.306988394324</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="6">
-        <v>44277.220075680241</v>
+        <v>44487.3285159507</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
         <v>3</v>
       </c>
       <c r="I41" s="6">
-        <v>44249.979688730557</v>
+        <v>44502.3747360329</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="I42" s="6">
-        <v>44322.573288355081</v>
+        <v>44533.98566068658</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2126,7 +2126,7 @@
         <v>3</v>
       </c>
       <c r="I43" s="6">
-        <v>44128.811365362366</v>
+        <v>44488.779943293725</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="6">
-        <v>44173.109570150169</v>
+        <v>44527.069898270303</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="6">
-        <v>44198.4614240257</v>
+        <v>44521.643493240037</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="I46" s="6">
-        <v>44287.914389380639</v>
+        <v>44491.352349463377</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="6">
-        <v>44166.107625968543</v>
+        <v>44510.717832002338</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,7 +2271,7 @@
         <v>4</v>
       </c>
       <c r="I48" s="6">
-        <v>44292.198117812695</v>
+        <v>44492.233221740855</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="6">
-        <v>44240.958154195105</v>
+        <v>44521.548306146884</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="I50" s="6">
-        <v>44179.632696685134</v>
+        <v>44512.136069916523</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="6">
-        <v>44224.954030028355</v>
+        <v>44500.849278952286</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
         <v>4</v>
       </c>
       <c r="I52" s="6">
-        <v>44174.762039353292</v>
+        <v>44498.171315551568</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="6">
-        <v>44199.206186179064</v>
+        <v>44485.07597405446</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="6">
-        <v>44259.019708119951</v>
+        <v>44482.853922032016</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="I55" s="6">
-        <v>44188.001280854136</v>
+        <v>44473.059420373873</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="6">
-        <v>44343.889685703849</v>
+        <v>44532.825130608297</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>4</v>
       </c>
       <c r="I57" s="6">
-        <v>44242.375158981595</v>
+        <v>44523.39204294236</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>3</v>
       </c>
       <c r="I58" s="6">
-        <v>44247.510854288499</v>
+        <v>44473.375025826106</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
         <v>4</v>
       </c>
       <c r="I59" s="6">
-        <v>44291.106469070095</v>
+        <v>44475.366747001906</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2616,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="I60" s="6">
-        <v>44192.121738901056</v>
+        <v>44476.006841058675</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>3</v>
       </c>
       <c r="I61" s="6">
-        <v>44141.465619838389</v>
+        <v>44526.74610053315</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="G1" t="str">
         <f ca="1">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Vincziczki Maximilián</v>
+        <v>Gózon Celesztin</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" ca="1" si="0">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Szilágyi Kökény</v>
+        <v>Vincziczki Surd</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Allegra</v>
+        <v>Szilágyi Melodi</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Deodát</v>
+        <v>Németh Szilamér</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Fortunát</v>
+        <v>Németh Pintyőke</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Ninett</v>
+        <v>Felföldi Pintyőke</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Vilibald</v>
+        <v>Berényi Surd</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Pintyőke</v>
+        <v>Gózon Szörénke</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Surd</v>
+        <v>Sárközi Kökény</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Deodát</v>
+        <v>Szilágyi Vilibald</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Deodát</v>
+        <v>Pintér Szilamér</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Surd</v>
+        <v>Ruzsinszki Celesztin</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Maximilián</v>
+        <v>Ruzsinszki Lizander</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Melodi</v>
+        <v>Németh Szörénke</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Reinhard</v>
+        <v>Gózon Maximilián</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2854,7 +2854,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Szörénke</v>
+        <v>Rácz Jarmilla</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Pintyőke</v>
+        <v>Vincziczki Reinhard</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2872,7 +2872,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Surd</v>
+        <v>Gózon Reinhard</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Kökény</v>
+        <v>Rácz Fortunát</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -2890,217 +2890,217 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Elina</v>
+        <v>Németh Kökény</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Pintyőke</v>
+        <v>Felföldi Elina</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Bereniké</v>
+        <v>Rácz Szilamér</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Szilamér</v>
+        <v>Pintér Zengő</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Pintyőke</v>
+        <v>Németh Allegra</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Pintyőke</v>
+        <v>Rácz Maximilián</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Allegra</v>
+        <v>Ruzsinszki Terestyén</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Allegra</v>
+        <v>Felföldi Terestyén</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Szörénke</v>
+        <v>Sárközi Szörénke</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Reinhard</v>
+        <v>Felföldi Zengő</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Zengő</v>
+        <v>Szilágyi Pintyőke</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Bereniké</v>
+        <v>Rácz Surd</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Szilamér</v>
+        <v>Sárközi Maximilián</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Melodi</v>
+        <v>Szilágyi Ninett</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Vilibald</v>
+        <v>Vincziczki Celesztin</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Vilibald</v>
+        <v>Ruzsinszki Kökény</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Maximilián</v>
+        <v>Sárközi Allegra</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Szilamér</v>
+        <v>Sárközi Zengő</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Fortunát</v>
+        <v>Németh Ninett</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Reinhard</v>
+        <v>Sárközi Kökény</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Ninett</v>
+        <v>Felföldi Lizander</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Vilibald</v>
+        <v>Pintér Kökény</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Zengő</v>
+        <v>Gózon Allegra</v>
       </c>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G43" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Zengő</v>
+        <v>Szilágyi Jarmilla</v>
       </c>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Pintyőke</v>
+        <v>Németh Deodát</v>
       </c>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Bereniké</v>
+        <v>Sárközi Melodi</v>
       </c>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Deodát</v>
+        <v>Gózon Surd</v>
       </c>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G47" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Lizander</v>
+        <v>Szilágyi Kökény</v>
       </c>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Reinhard</v>
+        <v>Sárközi Kökény</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Ninett</v>
+        <v>Gózon Szilamér</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Lizander</v>
+        <v>Berényi Maximilián</v>
       </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Pintyőke</v>
+        <v>Gózon Maximilián</v>
       </c>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G52" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Fortunát</v>
+        <v>Berényi Surd</v>
       </c>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G53" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Ninett</v>
+        <v>Gózon Zengő</v>
       </c>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Lizander</v>
+        <v>Rácz Kökény</v>
       </c>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G55" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Jarmilla</v>
+        <v>Vincziczki Deodát</v>
       </c>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
@@ -3112,385 +3112,385 @@
     <row r="57" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G57" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Zengő</v>
+        <v>Berényi Surd</v>
       </c>
     </row>
     <row r="58" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G58" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Szörénke</v>
+        <v>Rácz Deodát</v>
       </c>
     </row>
     <row r="59" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G59" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Szilamér</v>
+        <v>Gózon Elina</v>
       </c>
     </row>
     <row r="60" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G60" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Celesztin</v>
+        <v>Szilágyi Elina</v>
       </c>
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G61" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Lizander</v>
+        <v>Vincziczki Surd</v>
       </c>
     </row>
     <row r="62" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G62" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Maximilián</v>
+        <v>Berényi Kökény</v>
       </c>
     </row>
     <row r="63" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G63" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Bereniké</v>
+        <v>Szilágyi Szörénke</v>
       </c>
     </row>
     <row r="64" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G64" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Surd</v>
+        <v>Pintér Surd</v>
       </c>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G65" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Melodi</v>
+        <v>Vincziczki Celesztin</v>
       </c>
     </row>
     <row r="66" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G66" t="str">
         <f t="shared" ref="G66:G120" ca="1" si="1">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Sárközi Ninett</v>
+        <v>Vincziczki Terestyén</v>
       </c>
     </row>
     <row r="67" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G67" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Lizander</v>
+        <v>Sárközi Surd</v>
       </c>
     </row>
     <row r="68" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G68" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Ninett</v>
+        <v>Felföldi Ninett</v>
       </c>
     </row>
     <row r="69" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G69" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Vilibald</v>
+        <v>Sárközi Celesztin</v>
       </c>
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Lizander</v>
+        <v>Pintér Surd</v>
       </c>
     </row>
     <row r="71" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G71" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Ninett</v>
+        <v>Felföldi Deodát</v>
       </c>
     </row>
     <row r="72" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G72" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Maximilián</v>
+        <v>Pintér Terestyén</v>
       </c>
     </row>
     <row r="73" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G73" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Reinhard</v>
+        <v>Gózon Lizander</v>
       </c>
     </row>
     <row r="74" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G74" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Szilamér</v>
+        <v>Ruzsinszki Zengő</v>
       </c>
     </row>
     <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Szörénke</v>
+        <v>Ruzsinszki Terestyén</v>
       </c>
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Surd</v>
+        <v>Pintér Allegra</v>
       </c>
     </row>
     <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Kökény</v>
+        <v>Sárközi Elina</v>
       </c>
     </row>
     <row r="78" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G78" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Reinhard</v>
+        <v>Gózon Terestyén</v>
       </c>
     </row>
     <row r="79" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G79" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Allegra</v>
+        <v>Sárközi Celesztin</v>
       </c>
     </row>
     <row r="80" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G80" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Vilibald</v>
+        <v>Szilágyi Zengő</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Szilamér</v>
+        <v>Rácz Surd</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Vilibald</v>
+        <v>Sárközi Deodát</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Pintyőke</v>
+        <v>Berényi Kökény</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Melodi</v>
+        <v>Németh Vilibald</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Szörénke</v>
+        <v>Pintér Pintyőke</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Szilamér</v>
+        <v>Sárközi Kökény</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Maximilián</v>
+        <v>Gózon Szörénke</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Elina</v>
+        <v>Felföldi Terestyén</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Ninett</v>
+        <v>Németh Szilamér</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Elina</v>
+        <v>Szilágyi Deodát</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Deodát</v>
+        <v>Vincziczki Ninett</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Terestyén</v>
+        <v>Vincziczki Melodi</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Lizander</v>
+        <v>Felföldi Allegra</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Maximilián</v>
+        <v>Ruzsinszki Zengő</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Reinhard</v>
+        <v>Felföldi Maximilián</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Ninett</v>
+        <v>Felföldi Szörénke</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Celesztin</v>
+        <v>Pintér Reinhard</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Zengő</v>
+        <v>Rácz Melodi</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Deodát</v>
+        <v>Szilágyi Deodát</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Melodi</v>
+        <v>Vincziczki Deodát</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Pintyőke</v>
+        <v>Sárközi Kökény</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Allegra</v>
+        <v>Pintér Jarmilla</v>
       </c>
     </row>
     <row r="103" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G103" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Kökény</v>
+        <v>Gózon Elina</v>
       </c>
     </row>
     <row r="104" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G104" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Fortunát</v>
+        <v>Vincziczki Fortunát</v>
       </c>
     </row>
     <row r="105" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G105" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Ninett</v>
+        <v>Gózon Zengő</v>
       </c>
     </row>
     <row r="106" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G106" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Maximilián</v>
+        <v>Gózon Reinhard</v>
       </c>
     </row>
     <row r="107" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G107" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Vilibald</v>
+        <v>Pintér Maximilián</v>
       </c>
     </row>
     <row r="108" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G108" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Melodi</v>
+        <v>Rácz Allegra</v>
       </c>
     </row>
     <row r="109" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G109" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Bereniké</v>
+        <v>Ruzsinszki Celesztin</v>
       </c>
     </row>
     <row r="110" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G110" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Surd</v>
+        <v>Vincziczki Reinhard</v>
       </c>
     </row>
     <row r="111" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G111" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Deodát</v>
+        <v>Vincziczki Szörénke</v>
       </c>
     </row>
     <row r="112" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G112" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Szilamér</v>
+        <v>Szilágyi Surd</v>
       </c>
     </row>
     <row r="113" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G113" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Bereniké</v>
+        <v>Vincziczki Reinhard</v>
       </c>
     </row>
     <row r="114" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G114" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Vilibald</v>
+        <v>Felföldi Elina</v>
       </c>
     </row>
     <row r="115" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G115" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Elina</v>
+        <v>Szilágyi Lizander</v>
       </c>
     </row>
     <row r="116" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G116" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Pintyőke</v>
+        <v>Németh Reinhard</v>
       </c>
     </row>
     <row r="117" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G117" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Surd</v>
+        <v>Berényi Zengő</v>
       </c>
     </row>
     <row r="118" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G118" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Terestyén</v>
+        <v>Szilágyi Reinhard</v>
       </c>
     </row>
     <row r="119" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G119" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Vilibald</v>
+        <v>Sárközi Lizander</v>
       </c>
     </row>
     <row r="120" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G120" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Bereniké</v>
+        <v>Pintér Elina</v>
       </c>
     </row>
   </sheetData>
@@ -3502,7 +3502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9FB50B-CC00-457D-BC69-CBCBF715562E}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3513,626 +3515,626 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
-        <v>44075</v>
+        <v>44470</v>
       </c>
       <c r="B1" s="4">
         <f>A1</f>
-        <v>44075</v>
+        <v>44470</v>
       </c>
       <c r="E1" s="4">
         <f ca="1">RANDBETWEEN($B$1,$B$2)+RAND()</f>
-        <v>44154.883773988731</v>
+        <v>44491.072089168483</v>
       </c>
       <c r="F1" s="5">
         <f ca="1">E1</f>
-        <v>44154.883773988731</v>
+        <v>44491.072089168483</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>44347.999988425923</v>
+        <v>44533.999988425923</v>
       </c>
       <c r="B2" s="4">
         <f>A2</f>
-        <v>44347.999988425923</v>
+        <v>44533.999988425923</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" ref="E2:E61" ca="1" si="0">RANDBETWEEN($B$1,$B$2)+RAND()</f>
-        <v>44289.795374912901</v>
+        <v>44474.358557544307</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F61" ca="1" si="1">E2</f>
-        <v>44289.795374912901</v>
+        <v>44474.358557544307</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44093.769472536136</v>
+        <v>44533.169697061458</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44093.769472536136</v>
+        <v>44533.169697061458</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44255.998684138627</v>
+        <v>44514.638788785058</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44255.998684138627</v>
+        <v>44514.638788785058</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44181.450113663166</v>
+        <v>44490.030992222899</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44181.450113663166</v>
+        <v>44490.030992222899</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44306.136962662473</v>
+        <v>44470.915221044575</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44306.136962662473</v>
+        <v>44470.915221044575</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44120.880708739554</v>
+        <v>44501.349133187854</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44120.880708739554</v>
+        <v>44501.349133187854</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44306.818937934673</v>
+        <v>44504.397224937231</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44306.818937934673</v>
+        <v>44504.397224937231</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44202.439555648278</v>
+        <v>44533.775085548092</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44202.439555648278</v>
+        <v>44533.775085548092</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44121.280122860764</v>
+        <v>44525.949442777957</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44121.280122860764</v>
+        <v>44525.949442777957</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44160.165648241229</v>
+        <v>44472.72491700128</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44160.165648241229</v>
+        <v>44472.72491700128</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.109522642684</v>
+        <v>44476.091251426267</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.109522642684</v>
+        <v>44476.091251426267</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44146.602708106642</v>
+        <v>44527.087502448936</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44146.602708106642</v>
+        <v>44527.087502448936</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44097.796835087989</v>
+        <v>44532.67030632597</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44097.796835087989</v>
+        <v>44532.67030632597</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44107.700614050591</v>
+        <v>44474.622323501782</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44107.700614050591</v>
+        <v>44474.622323501782</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44189.012613774838</v>
+        <v>44484.578964792068</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44189.012613774838</v>
+        <v>44484.578964792068</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44241.021498457056</v>
+        <v>44505.366830174717</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44241.021498457056</v>
+        <v>44505.366830174717</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44204.01307922876</v>
+        <v>44472.603211046691</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44204.01307922876</v>
+        <v>44472.603211046691</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44242.923860598305</v>
+        <v>44471.926034489305</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44242.923860598305</v>
+        <v>44471.926034489305</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44182.65343816323</v>
+        <v>44499.592766250898</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44182.65343816323</v>
+        <v>44499.592766250898</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44132.161063206629</v>
+        <v>44475.834997330661</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44132.161063206629</v>
+        <v>44475.834997330661</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44195.997529548302</v>
+        <v>44531.869550931733</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44195.997529548302</v>
+        <v>44531.869550931733</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44179.25471622777</v>
+        <v>44505.855853511959</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44179.25471622777</v>
+        <v>44505.855853511959</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44306.003004764796</v>
+        <v>44520.064110747262</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44306.003004764796</v>
+        <v>44520.064110747262</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44292.903840019688</v>
+        <v>44519.94290759998</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44292.903840019688</v>
+        <v>44519.94290759998</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44311.358793914158</v>
+        <v>44530.646500699746</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44311.358793914158</v>
+        <v>44530.646500699746</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44329.7002804566</v>
+        <v>44513.656825692706</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44329.7002804566</v>
+        <v>44513.656825692706</v>
       </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44267.60320103282</v>
+        <v>44528.223381471755</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44267.60320103282</v>
+        <v>44528.223381471755</v>
       </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44130.006092122261</v>
+        <v>44481.21291073435</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44130.006092122261</v>
+        <v>44481.21291073435</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E30" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44146.840617648239</v>
+        <v>44500.067822962752</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44146.840617648239</v>
+        <v>44500.067822962752</v>
       </c>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E31" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44155.484353169639</v>
+        <v>44492.03152409679</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44155.484353169639</v>
+        <v>44492.03152409679</v>
       </c>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44221.700265049738</v>
+        <v>44533.646853886014</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44221.700265049738</v>
+        <v>44533.646853886014</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44111.653036146461</v>
+        <v>44484.945927144719</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44111.653036146461</v>
+        <v>44484.945927144719</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.078089582494</v>
+        <v>44494.766838014577</v>
       </c>
       <c r="F34" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.078089582494</v>
+        <v>44494.766838014577</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44167.157315318604</v>
+        <v>44516.996880608793</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44167.157315318604</v>
+        <v>44516.996880608793</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E36" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44136.28240850474</v>
+        <v>44530.330203046753</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44136.28240850474</v>
+        <v>44530.330203046753</v>
       </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E37" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44160.610989262641</v>
+        <v>44492.013635905627</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44160.610989262641</v>
+        <v>44492.013635905627</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44183.185226706286</v>
+        <v>44483.676016208847</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44183.185226706286</v>
+        <v>44483.676016208847</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E39" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44088.334322523282</v>
+        <v>44516.656761251448</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44088.334322523282</v>
+        <v>44516.656761251448</v>
       </c>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E40" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44257.521055500976</v>
+        <v>44505.661099444922</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44257.521055500976</v>
+        <v>44505.661099444922</v>
       </c>
     </row>
     <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44087.206715033215</v>
+        <v>44474.085522041139</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44087.206715033215</v>
+        <v>44474.085522041139</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E42" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44175.447977105548</v>
+        <v>44475.50352256804</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44175.447977105548</v>
+        <v>44475.50352256804</v>
       </c>
     </row>
     <row r="43" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E43" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44291.013345958294</v>
+        <v>44478.987801325806</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44291.013345958294</v>
+        <v>44478.987801325806</v>
       </c>
     </row>
     <row r="44" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E44" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44114.26938382088</v>
+        <v>44517.02193337489</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44114.26938382088</v>
+        <v>44517.02193337489</v>
       </c>
     </row>
     <row r="45" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E45" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44116.149883877741</v>
+        <v>44486.314449427162</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44116.149883877741</v>
+        <v>44486.314449427162</v>
       </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E46" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44284.390682756508</v>
+        <v>44486.96332655727</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44284.390682756508</v>
+        <v>44486.96332655727</v>
       </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44191.584597184577</v>
+        <v>44490.511229420343</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44191.584597184577</v>
+        <v>44490.511229420343</v>
       </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E48" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44134.442424413268</v>
+        <v>44472.609320137562</v>
       </c>
       <c r="F48" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44134.442424413268</v>
+        <v>44472.609320137562</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44292.01360449956</v>
+        <v>44514.294415140947</v>
       </c>
       <c r="F49" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44292.01360449956</v>
+        <v>44514.294415140947</v>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44113.560163197726</v>
+        <v>44519.572754615685</v>
       </c>
       <c r="F50" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44113.560163197726</v>
+        <v>44519.572754615685</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E51" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44156.267133971407</v>
+        <v>44499.705460554964</v>
       </c>
       <c r="F51" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44156.267133971407</v>
+        <v>44499.705460554964</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E52" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44139.929496993878</v>
+        <v>44510.306833793911</v>
       </c>
       <c r="F52" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44139.929496993878</v>
+        <v>44510.306833793911</v>
       </c>
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44120.709768544941</v>
+        <v>44529.784322780761</v>
       </c>
       <c r="F53" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44120.709768544941</v>
+        <v>44529.784322780761</v>
       </c>
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E54" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44229.769572995188</v>
+        <v>44490.143642021845</v>
       </c>
       <c r="F54" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44229.769572995188</v>
+        <v>44490.143642021845</v>
       </c>
     </row>
     <row r="55" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E55" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44291.142730122476</v>
+        <v>44496.176882813983</v>
       </c>
       <c r="F55" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44291.142730122476</v>
+        <v>44496.176882813983</v>
       </c>
     </row>
     <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E56" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44153.037774559176</v>
+        <v>44484.14339757798</v>
       </c>
       <c r="F56" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44153.037774559176</v>
+        <v>44484.14339757798</v>
       </c>
     </row>
     <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E57" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44082.230816574433</v>
+        <v>44475.967429796459</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44082.230816574433</v>
+        <v>44475.967429796459</v>
       </c>
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E58" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44187.478630070662</v>
+        <v>44504.930196077104</v>
       </c>
       <c r="F58" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44187.478630070662</v>
+        <v>44504.930196077104</v>
       </c>
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E59" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44335.52303630895</v>
+        <v>44530.789374860658</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44335.52303630895</v>
+        <v>44530.789374860658</v>
       </c>
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E60" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44190.846114945525</v>
+        <v>44472.501857533709</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44190.846114945525</v>
+        <v>44472.501857533709</v>
       </c>
     </row>
     <row r="61" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E61" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44345.110464196456</v>
+        <v>44482.46250212787</v>
       </c>
       <c r="F61" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44345.110464196456</v>
+        <v>44482.46250212787</v>
       </c>
     </row>
   </sheetData>
@@ -4145,7 +4147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58ADD0FC-5072-469C-88CD-500F5F08E611}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -5634,21 +5636,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010005E8C0DACDE33E40BC60C4A7B421D0DB" ma:contentTypeVersion="14" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="2ccb1f50ff8c2ae2e2332e3fac4317cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1cb6d7a-3261-4a52-912c-30bd985cd9a0" xmlns:ns4="2570eee2-52cd-4c6d-b9d4-12ed7ee7b87c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e29fd0fc1f13148ff6d3b0a1335d9761" ns3:_="" ns4:_="">
     <xsd:import namespace="e1cb6d7a-3261-4a52-912c-30bd985cd9a0"/>
@@ -5877,32 +5864,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4376DB1-7792-43C5-8AE8-8EEB9CB3E17A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312F9107-DD8E-4E22-938F-F1934A555547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2570eee2-52cd-4c6d-b9d4-12ed7ee7b87c"/>
-    <ds:schemaRef ds:uri="e1cb6d7a-3261-4a52-912c-30bd985cd9a0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398ABB07-9DD5-477B-82DC-28EB638FB6FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5919,4 +5896,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312F9107-DD8E-4E22-938F-F1934A555547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e1cb6d7a-3261-4a52-912c-30bd985cd9a0"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2570eee2-52cd-4c6d-b9d4-12ed7ee7b87c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4376DB1-7792-43C5-8AE8-8EEB9CB3E17A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed build version for production
</commit_message>
<xml_diff>
--- a/db-backup/MockData.xlsx
+++ b/db-backup/MockData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Egyetem_PTI\Diplomamunka\thesis-dms\db-backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{20C343D2-179B-4209-8BD7-964E79DDECA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{554B84A8-4EBB-4FF5-A5D6-4AA4735B7A66}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{20C343D2-179B-4209-8BD7-964E79DDECA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{ED1BC611-914A-4C23-94A3-8ABF752F4FE4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="24825" xr2:uid="{CCBAF8E0-E5E1-4B4B-975B-45441D02614E}"/>
   </bookViews>
@@ -880,11 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D87BECB-08DB-4F65-B57C-C5F108A9095E}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1015,7 @@
         <v>44513.343538625973</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>8094707763</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>44520.658584588135</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>8403042350</v>
       </c>
@@ -2246,7 +2245,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="7">
         <v>8713053299</v>
       </c>
       <c r="B48" s="2">
@@ -2390,7 +2389,7 @@
         <v>44498.171315551568</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>8805011634</v>
       </c>
@@ -2653,11 +2652,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I61" xr:uid="{0CC19ED8-7EBD-4E6A-966A-000B97AC08FD}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:I61">
       <sortCondition ref="A1"/>
     </sortState>
@@ -2692,7 +2686,7 @@
       </c>
       <c r="G1" t="str">
         <f ca="1">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Gózon Celesztin</v>
+        <v>Gózon Bereniké</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2704,7 +2698,7 @@
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" ca="1" si="0">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Vincziczki Surd</v>
+        <v>Sárközi Szörénke</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,7 +2710,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Melodi</v>
+        <v>Ruzsinszki Bereniké</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2728,7 +2722,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Szilamér</v>
+        <v>Berényi Terestyén</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2740,7 +2734,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Pintyőke</v>
+        <v>Sárközi Lizander</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2752,7 +2746,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Pintyőke</v>
+        <v>Felföldi Fortunát</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2764,7 +2758,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Surd</v>
+        <v>Rácz Vilibald</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2776,7 +2770,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Szörénke</v>
+        <v>Sárközi Fortunát</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,7 +2782,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Kökény</v>
+        <v>Vincziczki Fortunát</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2800,7 +2794,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Vilibald</v>
+        <v>Vincziczki Deodát</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2809,7 +2803,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Szilamér</v>
+        <v>Rácz Vilibald</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2818,7 +2812,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Celesztin</v>
+        <v>Pintér Celesztin</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2827,7 +2821,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Lizander</v>
+        <v>Berényi Szilamér</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2836,7 +2830,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Szörénke</v>
+        <v>Németh Surd</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2839,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Maximilián</v>
+        <v>Németh Bereniké</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2854,7 +2848,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Jarmilla</v>
+        <v>Gózon Deodát</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2863,7 +2857,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Reinhard</v>
+        <v>Szilágyi Ninett</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2872,7 +2866,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Reinhard</v>
+        <v>Ruzsinszki Celesztin</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -2881,7 +2875,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Fortunát</v>
+        <v>Rácz Elina</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -2890,607 +2884,607 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Kökény</v>
+        <v>Szilágyi Melodi</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Elina</v>
+        <v>Szilágyi Szilamér</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Szilamér</v>
+        <v>Vincziczki Ninett</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Zengő</v>
+        <v>Ruzsinszki Zengő</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Allegra</v>
+        <v>Ruzsinszki Melodi</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Maximilián</v>
+        <v>Ruzsinszki Lizander</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Terestyén</v>
+        <v>Berényi Kökény</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Terestyén</v>
+        <v>Felföldi Melodi</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Szörénke</v>
+        <v>Vincziczki Ninett</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Zengő</v>
+        <v>Berényi Zengő</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Pintyőke</v>
+        <v>Ruzsinszki Celesztin</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Surd</v>
+        <v>Pintér Terestyén</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Maximilián</v>
+        <v>Németh Fortunát</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Ninett</v>
+        <v>Németh Vilibald</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Celesztin</v>
+        <v>Gózon Bereniké</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Kökény</v>
+        <v>Ruzsinszki Allegra</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Allegra</v>
+        <v>Felföldi Deodát</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Zengő</v>
+        <v>Rácz Jarmilla</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Ninett</v>
+        <v>Sárközi Fortunát</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Kökény</v>
+        <v>Felföldi Vilibald</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Felföldi Lizander</v>
+        <v>Vincziczki Reinhard</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Kökény</v>
+        <v>Szilágyi Jarmilla</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Allegra</v>
+        <v>Szilágyi Deodát</v>
       </c>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G43" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Jarmilla</v>
+        <v>Vincziczki Kökény</v>
       </c>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Németh Deodát</v>
+        <v>Pintér Deodát</v>
       </c>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Melodi</v>
+        <v>Ruzsinszki Jarmilla</v>
       </c>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Surd</v>
+        <v>Pintér Celesztin</v>
       </c>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G47" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Kökény</v>
+        <v>Felföldi Bereniké</v>
       </c>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sárközi Kökény</v>
+        <v>Rácz Melodi</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Szilamér</v>
+        <v>Szilágyi Melodi</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Maximilián</v>
+        <v>Németh Jarmilla</v>
       </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Maximilián</v>
+        <v>Berényi Zengő</v>
       </c>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G52" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Surd</v>
+        <v>Pintér Pintyőke</v>
       </c>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G53" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Zengő</v>
+        <v>Németh Reinhard</v>
       </c>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Kökény</v>
+        <v>Pintér Celesztin</v>
       </c>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G55" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Deodát</v>
+        <v>Sárközi Maximilián</v>
       </c>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ruzsinszki Celesztin</v>
+        <v>Ruzsinszki Maximilián</v>
       </c>
     </row>
     <row r="57" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G57" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Surd</v>
+        <v>Németh Maximilián</v>
       </c>
     </row>
     <row r="58" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G58" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rácz Deodát</v>
+        <v>Rácz Vilibald</v>
       </c>
     </row>
     <row r="59" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G59" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gózon Elina</v>
+        <v>Szilágyi Elina</v>
       </c>
     </row>
     <row r="60" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G60" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Elina</v>
+        <v>Pintér Reinhard</v>
       </c>
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G61" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Surd</v>
+        <v>Berényi Fortunát</v>
       </c>
     </row>
     <row r="62" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G62" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berényi Kökény</v>
+        <v>Németh Lizander</v>
       </c>
     </row>
     <row r="63" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G63" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Szilágyi Szörénke</v>
+        <v>Szilágyi Kökény</v>
       </c>
     </row>
     <row r="64" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G64" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pintér Surd</v>
+        <v>Berényi Lizander</v>
       </c>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G65" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Vincziczki Celesztin</v>
+        <v>Ruzsinszki Kökény</v>
       </c>
     </row>
     <row r="66" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G66" t="str">
         <f t="shared" ref="G66:G120" ca="1" si="1">_xlfn.TEXTJOIN(" ",TRUE,INDEX($A$1:$A$10,RANDBETWEEN(1,ROWS($A$1:$A$10))), INDEX($B$1:$B$20,RANDBETWEEN(1,ROWS($B$1:$B$20))))</f>
-        <v>Vincziczki Terestyén</v>
+        <v>Berényi Terestyén</v>
       </c>
     </row>
     <row r="67" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G67" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Surd</v>
+        <v>Ruzsinszki Kökény</v>
       </c>
     </row>
     <row r="68" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G68" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Ninett</v>
+        <v>Rácz Zengő</v>
       </c>
     </row>
     <row r="69" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G69" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Celesztin</v>
+        <v>Vincziczki Szörénke</v>
       </c>
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Surd</v>
+        <v>Pintér Lizander</v>
       </c>
     </row>
     <row r="71" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G71" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Deodát</v>
+        <v>Vincziczki Lizander</v>
       </c>
     </row>
     <row r="72" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G72" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Terestyén</v>
+        <v>Németh Ninett</v>
       </c>
     </row>
     <row r="73" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G73" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Lizander</v>
+        <v>Felföldi Celesztin</v>
       </c>
     </row>
     <row r="74" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G74" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Zengő</v>
+        <v>Pintér Melodi</v>
       </c>
     </row>
     <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Terestyén</v>
+        <v>Berényi Ninett</v>
       </c>
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Allegra</v>
+        <v>Ruzsinszki Deodát</v>
       </c>
     </row>
     <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Elina</v>
+        <v>Pintér Celesztin</v>
       </c>
     </row>
     <row r="78" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G78" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Terestyén</v>
+        <v>Ruzsinszki Deodát</v>
       </c>
     </row>
     <row r="79" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G79" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Celesztin</v>
+        <v>Felföldi Szilamér</v>
       </c>
     </row>
     <row r="80" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G80" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Zengő</v>
+        <v>Vincziczki Pintyőke</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Surd</v>
+        <v>Ruzsinszki Reinhard</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Deodát</v>
+        <v>Rácz Vilibald</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Kökény</v>
+        <v>Rácz Szörénke</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Vilibald</v>
+        <v>Ruzsinszki Szilamér</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Pintyőke</v>
+        <v>Felföldi Jarmilla</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Kökény</v>
+        <v>Vincziczki Fortunát</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Szörénke</v>
+        <v>Ruzsinszki Surd</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Terestyén</v>
+        <v>Vincziczki Zengő</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Szilamér</v>
+        <v>Berényi Fortunát</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Deodát</v>
+        <v>Szilágyi Maximilián</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Ninett</v>
+        <v>Ruzsinszki Kökény</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Melodi</v>
+        <v>Vincziczki Maximilián</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Allegra</v>
+        <v>Pintér Lizander</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Zengő</v>
+        <v>Berényi Allegra</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Maximilián</v>
+        <v>Németh Reinhard</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Szörénke</v>
+        <v>Gózon Ninett</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Reinhard</v>
+        <v>Pintér Ninett</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Melodi</v>
+        <v>Gózon Lizander</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Deodát</v>
+        <v>Vincziczki Deodát</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Deodát</v>
+        <v>Ruzsinszki Jarmilla</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Kökény</v>
+        <v>Sárközi Elina</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Jarmilla</v>
+        <v>Gózon Terestyén</v>
       </c>
     </row>
     <row r="103" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G103" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Elina</v>
+        <v>Berényi Kökény</v>
       </c>
     </row>
     <row r="104" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G104" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Fortunát</v>
+        <v>Rácz Terestyén</v>
       </c>
     </row>
     <row r="105" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G105" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Zengő</v>
+        <v>Sárközi Reinhard</v>
       </c>
     </row>
     <row r="106" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G106" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gózon Reinhard</v>
+        <v>Sárközi Jarmilla</v>
       </c>
     </row>
     <row r="107" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G107" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Maximilián</v>
+        <v>Pintér Kökény</v>
       </c>
     </row>
     <row r="108" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G108" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Rácz Allegra</v>
+        <v>Felföldi Elina</v>
       </c>
     </row>
     <row r="109" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G109" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Ruzsinszki Celesztin</v>
+        <v>Berényi Celesztin</v>
       </c>
     </row>
     <row r="110" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G110" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Reinhard</v>
+        <v>Sárközi Jarmilla</v>
       </c>
     </row>
     <row r="111" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G111" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Szörénke</v>
+        <v>Sárközi Elina</v>
       </c>
     </row>
     <row r="112" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G112" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Surd</v>
+        <v>Berényi Maximilián</v>
       </c>
     </row>
     <row r="113" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G113" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Vincziczki Reinhard</v>
+        <v>Szilágyi Szilamér</v>
       </c>
     </row>
     <row r="114" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G114" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Felföldi Elina</v>
+        <v>Felföldi Fortunát</v>
       </c>
     </row>
     <row r="115" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G115" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Lizander</v>
+        <v>Vincziczki Zengő</v>
       </c>
     </row>
     <row r="116" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G116" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Németh Reinhard</v>
+        <v>Ruzsinszki Celesztin</v>
       </c>
     </row>
     <row r="117" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G117" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Berényi Zengő</v>
+        <v>Németh Pintyőke</v>
       </c>
     </row>
     <row r="118" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G118" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Szilágyi Reinhard</v>
+        <v>Rácz Kökény</v>
       </c>
     </row>
     <row r="119" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G119" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Sárközi Lizander</v>
+        <v>Gózon Celesztin</v>
       </c>
     </row>
     <row r="120" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G120" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Pintér Elina</v>
+        <v>Németh Maximilián</v>
       </c>
     </row>
   </sheetData>
@@ -3523,11 +3517,11 @@
       </c>
       <c r="E1" s="4">
         <f ca="1">RANDBETWEEN($B$1,$B$2)+RAND()</f>
-        <v>44491.072089168483</v>
+        <v>44477.627118550081</v>
       </c>
       <c r="F1" s="5">
         <f ca="1">E1</f>
-        <v>44491.072089168483</v>
+        <v>44477.627118550081</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3540,601 +3534,601 @@
       </c>
       <c r="E2" s="4">
         <f t="shared" ref="E2:E61" ca="1" si="0">RANDBETWEEN($B$1,$B$2)+RAND()</f>
-        <v>44474.358557544307</v>
+        <v>44522.725358077012</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F61" ca="1" si="1">E2</f>
-        <v>44474.358557544307</v>
+        <v>44522.725358077012</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44533.169697061458</v>
+        <v>44484.105147901682</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44533.169697061458</v>
+        <v>44484.105147901682</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44514.638788785058</v>
+        <v>44490.629784217119</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44514.638788785058</v>
+        <v>44490.629784217119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44490.030992222899</v>
+        <v>44515.108183332748</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44490.030992222899</v>
+        <v>44515.108183332748</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44470.915221044575</v>
+        <v>44521.277508460051</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44470.915221044575</v>
+        <v>44521.277508460051</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44501.349133187854</v>
+        <v>44505.861962555711</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44501.349133187854</v>
+        <v>44505.861962555711</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44504.397224937231</v>
+        <v>44480.984642707786</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44504.397224937231</v>
+        <v>44480.984642707786</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44533.775085548092</v>
+        <v>44476.820160995609</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44533.775085548092</v>
+        <v>44476.820160995609</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44525.949442777957</v>
+        <v>44522.527672134762</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44525.949442777957</v>
+        <v>44522.527672134762</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44472.72491700128</v>
+        <v>44499.337274713376</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44472.72491700128</v>
+        <v>44499.337274713376</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44476.091251426267</v>
+        <v>44479.186966176479</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44476.091251426267</v>
+        <v>44479.186966176479</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44527.087502448936</v>
+        <v>44515.712816292667</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44527.087502448936</v>
+        <v>44515.712816292667</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44532.67030632597</v>
+        <v>44470.492925638624</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44532.67030632597</v>
+        <v>44470.492925638624</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44474.622323501782</v>
+        <v>44521.346645640231</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44474.622323501782</v>
+        <v>44521.346645640231</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44484.578964792068</v>
+        <v>44485.0531150022</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44484.578964792068</v>
+        <v>44485.0531150022</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44505.366830174717</v>
+        <v>44524.821462017935</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44505.366830174717</v>
+        <v>44524.821462017935</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44472.603211046691</v>
+        <v>44523.805364208689</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44472.603211046691</v>
+        <v>44523.805364208689</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44471.926034489305</v>
+        <v>44480.113142205606</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44471.926034489305</v>
+        <v>44480.113142205606</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44499.592766250898</v>
+        <v>44496.820309591531</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44499.592766250898</v>
+        <v>44496.820309591531</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44475.834997330661</v>
+        <v>44533.39508174824</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44475.834997330661</v>
+        <v>44533.39508174824</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44531.869550931733</v>
+        <v>44507.018570410874</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44531.869550931733</v>
+        <v>44507.018570410874</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44505.855853511959</v>
+        <v>44470.319209498462</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44505.855853511959</v>
+        <v>44470.319209498462</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44520.064110747262</v>
+        <v>44506.777926336377</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44520.064110747262</v>
+        <v>44506.777926336377</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44519.94290759998</v>
+        <v>44513.33112494622</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44519.94290759998</v>
+        <v>44513.33112494622</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44530.646500699746</v>
+        <v>44481.045241046275</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44530.646500699746</v>
+        <v>44481.045241046275</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44513.656825692706</v>
+        <v>44527.838479611783</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44513.656825692706</v>
+        <v>44527.838479611783</v>
       </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44528.223381471755</v>
+        <v>44527.028070402986</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44528.223381471755</v>
+        <v>44527.028070402986</v>
       </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44481.21291073435</v>
+        <v>44533.146677602686</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44481.21291073435</v>
+        <v>44533.146677602686</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E30" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44500.067822962752</v>
+        <v>44504.72346441164</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44500.067822962752</v>
+        <v>44504.72346441164</v>
       </c>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E31" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44492.03152409679</v>
+        <v>44471.763615396289</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44492.03152409679</v>
+        <v>44471.763615396289</v>
       </c>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44533.646853886014</v>
+        <v>44527.56672190626</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44533.646853886014</v>
+        <v>44527.56672190626</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44484.945927144719</v>
+        <v>44524.884989370708</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44484.945927144719</v>
+        <v>44524.884989370708</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44494.766838014577</v>
+        <v>44501.144431149165</v>
       </c>
       <c r="F34" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44494.766838014577</v>
+        <v>44501.144431149165</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44516.996880608793</v>
+        <v>44484.301923365587</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44516.996880608793</v>
+        <v>44484.301923365587</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E36" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44530.330203046753</v>
+        <v>44493.583625980551</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44530.330203046753</v>
+        <v>44493.583625980551</v>
       </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E37" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44492.013635905627</v>
+        <v>44532.631911677374</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44492.013635905627</v>
+        <v>44532.631911677374</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44483.676016208847</v>
+        <v>44520.751088907527</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44483.676016208847</v>
+        <v>44520.751088907527</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E39" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44516.656761251448</v>
+        <v>44492.857326499441</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44516.656761251448</v>
+        <v>44492.857326499441</v>
       </c>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E40" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44505.661099444922</v>
+        <v>44487.178939610283</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44505.661099444922</v>
+        <v>44487.178939610283</v>
       </c>
     </row>
     <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44474.085522041139</v>
+        <v>44524.363870358276</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44474.085522041139</v>
+        <v>44524.363870358276</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E42" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44475.50352256804</v>
+        <v>44486.964061633116</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44475.50352256804</v>
+        <v>44486.964061633116</v>
       </c>
     </row>
     <row r="43" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E43" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44478.987801325806</v>
+        <v>44529.606649585578</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44478.987801325806</v>
+        <v>44529.606649585578</v>
       </c>
     </row>
     <row r="44" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E44" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44517.02193337489</v>
+        <v>44477.56644488532</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44517.02193337489</v>
+        <v>44477.56644488532</v>
       </c>
     </row>
     <row r="45" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E45" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44486.314449427162</v>
+        <v>44477.401111577405</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44486.314449427162</v>
+        <v>44477.401111577405</v>
       </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E46" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44486.96332655727</v>
+        <v>44510.724704908032</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44486.96332655727</v>
+        <v>44510.724704908032</v>
       </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44490.511229420343</v>
+        <v>44486.275457636184</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44490.511229420343</v>
+        <v>44486.275457636184</v>
       </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E48" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44472.609320137562</v>
+        <v>44533.694377436987</v>
       </c>
       <c r="F48" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44472.609320137562</v>
+        <v>44533.694377436987</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44514.294415140947</v>
+        <v>44475.926013949422</v>
       </c>
       <c r="F49" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44514.294415140947</v>
+        <v>44475.926013949422</v>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44519.572754615685</v>
+        <v>44511.563194282659</v>
       </c>
       <c r="F50" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44519.572754615685</v>
+        <v>44511.563194282659</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E51" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44499.705460554964</v>
+        <v>44520.399667781239</v>
       </c>
       <c r="F51" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44499.705460554964</v>
+        <v>44520.399667781239</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E52" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44510.306833793911</v>
+        <v>44506.284972066729</v>
       </c>
       <c r="F52" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44510.306833793911</v>
+        <v>44506.284972066729</v>
       </c>
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44529.784322780761</v>
+        <v>44519.226643853937</v>
       </c>
       <c r="F53" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44529.784322780761</v>
+        <v>44519.226643853937</v>
       </c>
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E54" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44490.143642021845</v>
+        <v>44518.859043154138</v>
       </c>
       <c r="F54" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44490.143642021845</v>
+        <v>44518.859043154138</v>
       </c>
     </row>
     <row r="55" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E55" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44496.176882813983</v>
+        <v>44485.734857421419</v>
       </c>
       <c r="F55" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44496.176882813983</v>
+        <v>44485.734857421419</v>
       </c>
     </row>
     <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E56" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44484.14339757798</v>
+        <v>44476.910014841458</v>
       </c>
       <c r="F56" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44484.14339757798</v>
+        <v>44476.910014841458</v>
       </c>
     </row>
     <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E57" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44475.967429796459</v>
+        <v>44473.441131635846</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44475.967429796459</v>
+        <v>44473.441131635846</v>
       </c>
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E58" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44504.930196077104</v>
+        <v>44499.063274954511</v>
       </c>
       <c r="F58" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44504.930196077104</v>
+        <v>44499.063274954511</v>
       </c>
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E59" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44530.789374860658</v>
+        <v>44532.099300044581</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44530.789374860658</v>
+        <v>44532.099300044581</v>
       </c>
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E60" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44472.501857533709</v>
+        <v>44489.235890482953</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44472.501857533709</v>
+        <v>44489.235890482953</v>
       </c>
     </row>
     <row r="61" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E61" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44482.46250212787</v>
+        <v>44516.213865081736</v>
       </c>
       <c r="F61" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44482.46250212787</v>
+        <v>44516.213865081736</v>
       </c>
     </row>
   </sheetData>
@@ -5901,15 +5895,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312F9107-DD8E-4E22-938F-F1934A555547}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e1cb6d7a-3261-4a52-912c-30bd985cd9a0"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2570eee2-52cd-4c6d-b9d4-12ed7ee7b87c"/>
+    <ds:schemaRef ds:uri="e1cb6d7a-3261-4a52-912c-30bd985cd9a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>